<commit_message>
added pdf preview, separator, passward protection
</commit_message>
<xml_diff>
--- a/Interactive Design Phase 2 APS efforts.xlsx
+++ b/Interactive Design Phase 2 APS efforts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Interactive Designer\current working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Interactive Designer\ID Phase 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DA77E3-51E1-4DD4-B9FA-FE4BDA45447F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE860225-B5A2-492F-892E-280F3EA87799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Latest Version" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="237">
   <si>
     <t>Phase-wise</t>
   </si>
@@ -975,6 +975,21 @@
     <t>Could you please elaborate on where you are noticing complexity during the development of simple static templates?
 - Are there specific features or design tools that are not user-friendly?
 - Understanding this will help us improve the overall workflow and simplify the experience for end users.</t>
+  </si>
+  <si>
+    <t>Text Wrap they want. Means if I fixed height in 2 column news format then extra text will automatically shifts or comes in next column.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mouse movement. Like I can move image, table, elements by using mouse. </t>
+  </si>
+  <si>
+    <t>resizing of elemnts through mouse want to implement.</t>
+  </si>
+  <si>
+    <t>Going only at end, after dragging apend only at end. Global scripting issue as per my opinion.</t>
+  </si>
+  <si>
+    <t>reposition of elemetgs in print preview. Elements position can be adjusted before printing. Only for printing purpose will not update in editor.</t>
   </si>
 </sst>
 </file>
@@ -18719,8 +18734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N1048"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B22" sqref="A22:XFD22"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -18837,7 +18852,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="99" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="G3" s="90" t="s">
         <v>152</v>
@@ -18849,7 +18864,7 @@
         <v>2</v>
       </c>
       <c r="J3" s="87" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="K3" s="11">
         <v>2</v>
@@ -18991,7 +19006,7 @@
       </c>
       <c r="E7" s="83"/>
       <c r="F7" s="100" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="G7" s="93" t="s">
         <v>154</v>
@@ -19001,6 +19016,9 @@
       </c>
       <c r="I7" s="10">
         <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>233</v>
       </c>
       <c r="K7" s="11">
         <v>2</v>
@@ -19553,7 +19571,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="87" t="s">
-        <v>205</v>
+        <v>234</v>
       </c>
       <c r="K22" s="11">
         <v>2</v>
@@ -20446,7 +20464,7 @@
       </c>
       <c r="E47" s="82"/>
       <c r="F47" s="100" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="G47" s="60" t="s">
         <v>156</v>
@@ -20458,7 +20476,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="87" t="s">
-        <v>183</v>
+        <v>235</v>
       </c>
       <c r="K47" s="11">
         <v>2</v>
@@ -21048,7 +21066,7 @@
       <c r="D63" s="56"/>
       <c r="E63" s="83"/>
       <c r="F63" s="99" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="G63" s="93" t="s">
         <v>156</v>
@@ -21060,7 +21078,7 @@
         <v>2</v>
       </c>
       <c r="J63" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="K63" s="11">
         <v>2</v>
@@ -26432,10 +26450,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D3E457-9EF0-4080-8E3A-86582F20D6ED}">
-  <dimension ref="A2:L7"/>
+  <dimension ref="A2:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView zoomScale="155" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26443,11 +26461,11 @@
     <col min="3" max="3" width="35.5546875" customWidth="1"/>
     <col min="4" max="4" width="51.33203125" customWidth="1"/>
     <col min="6" max="6" width="26.44140625" customWidth="1"/>
-    <col min="7" max="7" width="41.44140625" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="53.88671875" customWidth="1"/>
+    <col min="15" max="15" width="41.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
@@ -26465,9 +26483,6 @@
       </c>
       <c r="F2" s="99" t="s">
         <v>157</v>
-      </c>
-      <c r="G2" s="87" t="s">
-        <v>223</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>226</v>
@@ -26475,8 +26490,11 @@
       <c r="J2" s="87"/>
       <c r="K2" s="11"/>
       <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O2" s="87" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
@@ -26499,7 +26517,7 @@
       <c r="K3" s="11"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -26516,17 +26534,17 @@
       <c r="F4" s="99" t="s">
         <v>166</v>
       </c>
-      <c r="G4" s="87" t="s">
-        <v>205</v>
-      </c>
       <c r="H4" s="9" t="s">
         <v>231</v>
       </c>
       <c r="J4" s="87"/>
       <c r="K4" s="11"/>
       <c r="L4" s="12"/>
-    </row>
-    <row r="5" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O4" s="87" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>86</v>
       </c>
@@ -26543,17 +26561,17 @@
       <c r="F5" s="100" t="s">
         <v>155</v>
       </c>
-      <c r="G5" s="87" t="s">
-        <v>183</v>
-      </c>
       <c r="H5" s="44" t="s">
         <v>228</v>
       </c>
       <c r="J5" s="87"/>
       <c r="K5" s="11"/>
       <c r="L5" s="12"/>
-    </row>
-    <row r="6" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O5" s="87" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>86</v>
       </c>
@@ -26568,16 +26586,16 @@
       <c r="F6" s="99" t="s">
         <v>157</v>
       </c>
-      <c r="G6" t="s">
-        <v>222</v>
-      </c>
       <c r="H6" s="44" t="s">
         <v>227</v>
       </c>
       <c r="K6" s="11"/>
       <c r="L6" s="12"/>
-    </row>
-    <row r="7" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>86</v>
       </c>
@@ -26594,14 +26612,14 @@
       <c r="F7" s="99" t="s">
         <v>157</v>
       </c>
-      <c r="G7" t="s">
-        <v>221</v>
-      </c>
       <c r="H7" s="9" t="s">
         <v>230</v>
       </c>
       <c r="K7" s="11"/>
       <c r="L7" s="12"/>
+      <c r="O7" t="s">
+        <v>221</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>